<commit_message>
Refactor Excel and XML handling in parsers; update header management and improve error logging
</commit_message>
<xml_diff>
--- a/func/templates/anexa.xlsx
+++ b/func/templates/anexa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\AppData\Roaming\QGIS\QGIS3\profiles\default\python\plugins\stalpi_assist_buttons\func\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71726377-4BF2-4A1F-B122-BE7C77165E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D2D405-9677-4D91-9B9E-D5271ABEBB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="815" firstSheet="3" activeTab="9" xr2:uid="{161416AC-371D-4DC7-8579-2717821BF42C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="815" firstSheet="3" activeTab="8" xr2:uid="{161416AC-371D-4DC7-8579-2717821BF42C}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="2" r:id="rId1"/>
@@ -4358,7 +4358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFEE384-6BDD-4738-B9A3-37CE1F7005EF}">
   <dimension ref="A2:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -4523,10 +4523,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:AA235"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4692,705 +4692,6 @@
       <c r="AA2" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="3"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="3"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="3"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="3"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="3"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="3"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="3"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="3"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="3"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="3"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="3"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="3"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="3"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="3"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="3"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="3"/>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="3"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="3"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="3"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="3"/>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="3"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="3"/>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="3"/>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="3"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="3"/>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="3"/>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="3"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="3"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="3"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="3"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="3"/>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="3"/>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="3"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="3"/>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="3"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="3"/>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="3"/>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="3"/>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="3"/>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="3"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="3"/>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="3"/>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="3"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="3"/>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="3"/>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="3"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="3"/>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="3"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="3"/>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="3"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="3"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="3"/>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="3"/>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="3"/>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="3"/>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="3"/>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="3"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="3"/>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="3"/>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="3"/>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="3"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="3"/>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" s="3"/>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="3"/>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" s="3"/>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="3"/>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="3"/>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170" s="3"/>
-    </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="3"/>
-    </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="3"/>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" s="3"/>
-    </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174" s="3"/>
-    </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175" s="3"/>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176" s="3"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="3"/>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="3"/>
-    </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179" s="3"/>
-    </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="3"/>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="3"/>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="3"/>
-    </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" s="3"/>
-    </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" s="3"/>
-    </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185" s="3"/>
-    </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="3"/>
-    </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B187" s="3"/>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188" s="3"/>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189" s="3"/>
-    </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190" s="3"/>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B191" s="3"/>
-    </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192" s="3"/>
-    </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B193" s="3"/>
-    </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B194" s="3"/>
-    </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B195" s="3"/>
-    </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B196" s="3"/>
-    </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B197" s="3"/>
-    </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B198" s="3"/>
-    </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B199" s="3"/>
-    </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B200" s="3"/>
-    </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B201" s="3"/>
-    </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B202" s="3"/>
-    </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B203" s="3"/>
-    </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B204" s="3"/>
-    </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B205" s="3"/>
-    </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B206" s="3"/>
-    </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B207" s="3"/>
-    </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B208" s="3"/>
-    </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B209" s="3"/>
-    </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B210" s="3"/>
-    </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B211" s="3"/>
-    </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B212" s="3"/>
-    </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B213" s="3"/>
-    </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B214" s="3"/>
-    </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B215" s="3"/>
-    </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B216" s="3"/>
-    </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B217" s="3"/>
-    </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B218" s="3"/>
-    </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B219" s="3"/>
-    </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B220" s="3"/>
-    </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B221" s="3"/>
-    </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B222" s="3"/>
-    </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B223" s="3"/>
-    </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B224" s="3"/>
-    </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B225" s="3"/>
-    </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B226" s="3"/>
-    </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B227" s="3"/>
-    </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B228" s="3"/>
-    </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B229" s="3"/>
-    </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B230" s="3"/>
-    </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B231" s="3"/>
-    </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B232" s="3"/>
-    </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B233" s="3"/>
-    </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B234" s="3"/>
-    </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B235" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8340,10 +7641,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:AF101"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8566,300 +7867,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="3"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="H3:J3"/>
@@ -8876,10 +7883,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:AB231"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9062,693 +8069,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="3"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="3"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="3"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="3"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="3"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="3"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="3"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="3"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="3"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="3"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="3"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="3"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="3"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="3"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="3"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="3"/>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="3"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="3"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="3"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="3"/>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="3"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="3"/>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="3"/>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="3"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="3"/>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="3"/>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="3"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="3"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="3"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="3"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="3"/>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="3"/>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="3"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="3"/>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="3"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="3"/>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="3"/>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="3"/>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="3"/>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="3"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="3"/>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="3"/>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="3"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="3"/>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="3"/>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="3"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="3"/>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="3"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="3"/>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="3"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="3"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="3"/>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="3"/>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="3"/>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="3"/>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="3"/>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="3"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="3"/>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="3"/>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="3"/>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="3"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="3"/>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" s="3"/>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="3"/>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" s="3"/>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="3"/>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="3"/>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170" s="3"/>
-    </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="3"/>
-    </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="3"/>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" s="3"/>
-    </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174" s="3"/>
-    </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175" s="3"/>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176" s="3"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="3"/>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="3"/>
-    </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179" s="3"/>
-    </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="3"/>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="3"/>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="3"/>
-    </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" s="3"/>
-    </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" s="3"/>
-    </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185" s="3"/>
-    </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="3"/>
-    </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B187" s="3"/>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188" s="3"/>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189" s="3"/>
-    </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190" s="3"/>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B191" s="3"/>
-    </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192" s="3"/>
-    </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B193" s="3"/>
-    </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B194" s="3"/>
-    </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B195" s="3"/>
-    </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B196" s="3"/>
-    </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B197" s="3"/>
-    </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B198" s="3"/>
-    </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B199" s="3"/>
-    </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B200" s="3"/>
-    </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B201" s="3"/>
-    </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B202" s="3"/>
-    </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B203" s="3"/>
-    </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B204" s="3"/>
-    </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B205" s="3"/>
-    </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B206" s="3"/>
-    </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B207" s="3"/>
-    </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B208" s="3"/>
-    </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B209" s="3"/>
-    </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B210" s="3"/>
-    </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B211" s="3"/>
-    </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B212" s="3"/>
-    </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B213" s="3"/>
-    </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B214" s="3"/>
-    </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B215" s="3"/>
-    </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B216" s="3"/>
-    </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B217" s="3"/>
-    </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B218" s="3"/>
-    </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B219" s="3"/>
-    </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B220" s="3"/>
-    </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B221" s="3"/>
-    </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B222" s="3"/>
-    </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B223" s="3"/>
-    </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B224" s="3"/>
-    </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B225" s="3"/>
-    </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B226" s="3"/>
-    </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B227" s="3"/>
-    </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B228" s="3"/>
-    </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B229" s="3"/>
-    </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B230" s="3"/>
-    </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B231" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H2:J2"/>

</xml_diff>